<commit_message>
Poll Passive Rewards (DigiPogs)
</commit_message>
<xml_diff>
--- a/basicjavascript.xlsx
+++ b/basicjavascript.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RRorrer\Documents\GitHub\Formbar.js\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\APlitt\Documents\ProgrammingGitHub2024\Formbar.js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B2BAF2-6EA2-4153-9FFC-4945B24527FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBCD9B-8D66-4C10-ACB9-22048EF64AA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="104">
   <si>
     <t>Question</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>Good, Meh, Confused, Upset</t>
+  </si>
+  <si>
+    <t>Weights</t>
+  </si>
+  <si>
+    <t>0.9, 1.1</t>
+  </si>
+  <si>
+    <t>0.9, 1.0, 1.1, 1.2</t>
   </si>
 </sst>
 </file>
@@ -684,10 +693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,7 +707,7 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -714,8 +723,11 @@
       <c r="E1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -731,8 +743,11 @@
       <c r="E2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -743,7 +758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -754,7 +769,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -770,11 +785,14 @@
       <c r="E5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
   </sheetData>
@@ -1197,12 +1215,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1384,15 +1399,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A2703C-FBA4-45C7-94E2-5BD99335F262}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78BD9466-AC2E-44D1-A6E0-91F63F9F04EC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cc9255bc-4d99-4f42-bba5-857cbcc6e725"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1416,17 +1442,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78BD9466-AC2E-44D1-A6E0-91F63F9F04EC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A2703C-FBA4-45C7-94E2-5BD99335F262}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cc9255bc-4d99-4f42-bba5-857cbcc6e725"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>